<commit_message>
Commit all files for Scientific Reports
</commit_message>
<xml_diff>
--- a/appendixTables.xlsx
+++ b/appendixTables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table_PredatorAbundances" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -566,6 +566,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10130,8 +10133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10199,28 +10202,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="8">
-        <v>275</v>
+        <v>695</v>
       </c>
       <c r="C3" s="8">
-        <v>275</v>
-      </c>
-      <c r="D3" s="8">
-        <v>28</v>
-      </c>
-      <c r="E3" s="8">
-        <v>28</v>
-      </c>
-      <c r="F3" s="8">
-        <v>34</v>
-      </c>
-      <c r="G3" s="8">
-        <v>27</v>
-      </c>
-      <c r="H3" s="8">
-        <v>22</v>
-      </c>
-      <c r="I3" s="8">
-        <v>22</v>
+        <v>695</v>
+      </c>
+      <c r="D3" s="25">
+        <v>28.044265530000001</v>
+      </c>
+      <c r="E3" s="25">
+        <v>27.85136412</v>
+      </c>
+      <c r="F3" s="25">
+        <v>34.106625190000003</v>
+      </c>
+      <c r="G3" s="25">
+        <v>26.567002030000001</v>
+      </c>
+      <c r="H3" s="25">
+        <v>95.557930839999997</v>
+      </c>
+      <c r="I3" s="25">
+        <v>96.885524899999993</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -10228,28 +10231,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="8">
-        <v>468</v>
+        <v>949</v>
       </c>
       <c r="C4" s="8">
-        <v>468</v>
-      </c>
-      <c r="D4" s="8">
-        <v>40</v>
-      </c>
-      <c r="E4" s="8">
-        <v>38</v>
-      </c>
-      <c r="F4" s="8">
-        <v>50</v>
-      </c>
-      <c r="G4" s="8">
-        <v>47</v>
-      </c>
-      <c r="H4" s="8">
-        <v>96</v>
-      </c>
-      <c r="I4" s="8">
-        <v>97</v>
+        <v>949</v>
+      </c>
+      <c r="D4" s="25">
+        <v>40.374197969999997</v>
+      </c>
+      <c r="E4" s="25">
+        <v>37.64431759</v>
+      </c>
+      <c r="F4" s="25">
+        <v>50.485769570000002</v>
+      </c>
+      <c r="G4" s="25">
+        <v>46.830284919999997</v>
+      </c>
+      <c r="H4" s="25">
+        <v>133.42736669999999</v>
+      </c>
+      <c r="I4" s="25">
+        <v>125.8213997</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -10257,28 +10260,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="8">
-        <v>702</v>
+        <v>1208</v>
       </c>
       <c r="C5" s="8">
-        <v>702</v>
-      </c>
-      <c r="D5" s="8">
-        <v>50</v>
-      </c>
-      <c r="E5" s="8">
-        <v>45</v>
-      </c>
-      <c r="F5" s="8">
-        <v>73</v>
-      </c>
-      <c r="G5" s="8">
-        <v>62</v>
-      </c>
-      <c r="H5" s="8">
-        <v>133</v>
-      </c>
-      <c r="I5" s="8">
-        <v>126</v>
+        <v>1208</v>
+      </c>
+      <c r="D5" s="25">
+        <v>50.046737380000003</v>
+      </c>
+      <c r="E5" s="25">
+        <v>45.300896129999998</v>
+      </c>
+      <c r="F5" s="25">
+        <v>73.059647229999996</v>
+      </c>
+      <c r="G5" s="25">
+        <v>62.151043860000001</v>
+      </c>
+      <c r="H5" s="25">
+        <v>182.09008589999999</v>
+      </c>
+      <c r="I5" s="25">
+        <v>152.0571917</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -10286,28 +10289,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="8">
-        <v>952</v>
+        <v>1455</v>
       </c>
       <c r="C6" s="8">
-        <v>952</v>
-      </c>
-      <c r="D6" s="8">
-        <v>58</v>
-      </c>
-      <c r="E6" s="8">
-        <v>51</v>
-      </c>
-      <c r="F6" s="8">
-        <v>103</v>
-      </c>
-      <c r="G6" s="8">
-        <v>72</v>
-      </c>
-      <c r="H6" s="8">
-        <v>182</v>
-      </c>
-      <c r="I6" s="8">
-        <v>152</v>
+        <v>1455</v>
+      </c>
+      <c r="D6" s="25">
+        <v>57.634615009999997</v>
+      </c>
+      <c r="E6" s="25">
+        <v>51.287159119999998</v>
+      </c>
+      <c r="F6" s="25">
+        <v>102.5661152</v>
+      </c>
+      <c r="G6" s="25">
+        <v>72.305172119999995</v>
+      </c>
+      <c r="H6" s="25">
+        <v>241.4814331</v>
+      </c>
+      <c r="I6" s="25">
+        <v>174.91601019999999</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -10315,28 +10318,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="9">
-        <v>1218</v>
+        <v>1682</v>
       </c>
       <c r="C7" s="9">
-        <v>1218</v>
-      </c>
-      <c r="D7" s="8">
-        <v>64</v>
-      </c>
-      <c r="E7" s="8">
-        <v>56</v>
-      </c>
-      <c r="F7" s="8">
-        <v>139</v>
-      </c>
-      <c r="G7" s="8">
-        <v>79</v>
-      </c>
-      <c r="H7" s="8">
-        <v>241</v>
-      </c>
-      <c r="I7" s="8">
-        <v>175</v>
+        <v>1682</v>
+      </c>
+      <c r="D7" s="25">
+        <v>63.587124940000002</v>
+      </c>
+      <c r="E7" s="25">
+        <v>55.967493079999997</v>
+      </c>
+      <c r="F7" s="25">
+        <v>138.57399240000001</v>
+      </c>
+      <c r="G7" s="25">
+        <v>78.611853879999998</v>
+      </c>
+      <c r="H7" s="25">
+        <v>309.57191410000001</v>
+      </c>
+      <c r="I7" s="25">
+        <v>194.28571410000001</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -10344,28 +10347,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="9">
-        <v>1460</v>
+        <v>1881</v>
       </c>
       <c r="C8" s="9">
-        <v>1460</v>
-      </c>
-      <c r="D8" s="8">
-        <v>68</v>
-      </c>
-      <c r="E8" s="8">
-        <v>60</v>
-      </c>
-      <c r="F8" s="8">
-        <v>179</v>
-      </c>
-      <c r="G8" s="8">
-        <v>82</v>
-      </c>
-      <c r="H8" s="8">
-        <v>310</v>
-      </c>
-      <c r="I8" s="8">
-        <v>194</v>
+        <v>1881</v>
+      </c>
+      <c r="D8" s="25">
+        <v>68.256727729999994</v>
+      </c>
+      <c r="E8" s="25">
+        <v>59.626792049999999</v>
+      </c>
+      <c r="F8" s="25">
+        <v>179.00744639999999</v>
+      </c>
+      <c r="G8" s="25">
+        <v>82.396612500000003</v>
+      </c>
+      <c r="H8" s="25">
+        <v>382.25715939999998</v>
+      </c>
+      <c r="I8" s="25">
+        <v>210.37353239999999</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -10373,28 +10376,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="9">
-        <v>1678</v>
+        <v>2051</v>
       </c>
       <c r="C9" s="9">
-        <v>1678</v>
-      </c>
-      <c r="D9" s="8">
-        <v>72</v>
-      </c>
-      <c r="E9" s="8">
-        <v>62</v>
-      </c>
-      <c r="F9" s="8">
-        <v>220</v>
-      </c>
-      <c r="G9" s="8">
-        <v>85</v>
-      </c>
-      <c r="H9" s="8">
-        <v>382</v>
-      </c>
-      <c r="I9" s="8">
-        <v>210</v>
+        <v>2051</v>
+      </c>
+      <c r="D9" s="25">
+        <v>71.919920300000001</v>
+      </c>
+      <c r="E9" s="25">
+        <v>62.487799209999999</v>
+      </c>
+      <c r="F9" s="25">
+        <v>220.37942509999999</v>
+      </c>
+      <c r="G9" s="25">
+        <v>84.625488919999995</v>
+      </c>
+      <c r="H9" s="25">
+        <v>454.16698639999998</v>
+      </c>
+      <c r="I9" s="25">
+        <v>223.54060039999999</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -10402,28 +10405,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="9">
-        <v>1880</v>
+        <v>2194</v>
       </c>
       <c r="C10" s="9">
-        <v>1880</v>
-      </c>
-      <c r="D10" s="8">
-        <v>75</v>
-      </c>
-      <c r="E10" s="8">
-        <v>65</v>
-      </c>
-      <c r="F10" s="8">
-        <v>259</v>
-      </c>
-      <c r="G10" s="8">
-        <v>86</v>
-      </c>
-      <c r="H10" s="8">
-        <v>454</v>
-      </c>
-      <c r="I10" s="8">
-        <v>224</v>
+        <v>2194</v>
+      </c>
+      <c r="D10" s="25">
+        <v>74.793607949999995</v>
+      </c>
+      <c r="E10" s="25">
+        <v>64.724665349999995</v>
+      </c>
+      <c r="F10" s="25">
+        <v>258.8740244</v>
+      </c>
+      <c r="G10" s="25">
+        <v>85.924306060000006</v>
+      </c>
+      <c r="H10" s="25">
+        <v>520.15296609999996</v>
+      </c>
+      <c r="I10" s="25">
+        <v>234.1998294</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -10431,28 +10434,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="9">
-        <v>2049</v>
+        <v>2311</v>
       </c>
       <c r="C11" s="9">
-        <v>2049</v>
-      </c>
-      <c r="D11" s="8">
-        <v>77</v>
-      </c>
-      <c r="E11" s="8">
-        <v>66</v>
-      </c>
-      <c r="F11" s="8">
-        <v>292</v>
-      </c>
-      <c r="G11" s="8">
-        <v>87</v>
-      </c>
-      <c r="H11" s="8">
-        <v>520</v>
-      </c>
-      <c r="I11" s="8">
-        <v>234</v>
+        <v>2311</v>
+      </c>
+      <c r="D11" s="25">
+        <v>77.047947710000003</v>
+      </c>
+      <c r="E11" s="25">
+        <v>66.473549509999998</v>
+      </c>
+      <c r="F11" s="25">
+        <v>291.65095609999997</v>
+      </c>
+      <c r="G11" s="25">
+        <v>86.676644620000005</v>
+      </c>
+      <c r="H11" s="25">
+        <v>576.65154749999999</v>
+      </c>
+      <c r="I11" s="25">
+        <v>242.7579796</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -10460,28 +10463,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="9">
-        <v>2202</v>
+        <v>2406</v>
       </c>
       <c r="C12" s="9">
-        <v>2202</v>
-      </c>
-      <c r="D12" s="8">
-        <v>79</v>
-      </c>
-      <c r="E12" s="8">
-        <v>68</v>
-      </c>
-      <c r="F12" s="8">
-        <v>318</v>
-      </c>
-      <c r="G12" s="8">
-        <v>87</v>
-      </c>
-      <c r="H12" s="8">
-        <v>577</v>
-      </c>
-      <c r="I12" s="8">
-        <v>243</v>
+        <v>2406</v>
+      </c>
+      <c r="D12" s="25">
+        <v>78.816423760000006</v>
+      </c>
+      <c r="E12" s="25">
+        <v>67.84090707</v>
+      </c>
+      <c r="F12" s="25">
+        <v>317.51654139999999</v>
+      </c>
+      <c r="G12" s="25">
+        <v>87.110953739999999</v>
+      </c>
+      <c r="H12" s="25">
+        <v>622.22839299999998</v>
+      </c>
+      <c r="I12" s="25">
+        <v>249.58627340000001</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -10489,28 +10492,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="9">
-        <v>2307</v>
+        <v>2482</v>
       </c>
       <c r="C13" s="9">
-        <v>2307</v>
-      </c>
-      <c r="D13" s="8">
-        <v>80</v>
-      </c>
-      <c r="E13" s="8">
-        <v>69</v>
-      </c>
-      <c r="F13" s="8">
-        <v>318</v>
-      </c>
-      <c r="G13" s="8">
-        <v>87</v>
-      </c>
-      <c r="H13" s="8">
-        <v>622</v>
-      </c>
-      <c r="I13" s="8">
-        <v>250</v>
+        <v>2482</v>
+      </c>
+      <c r="D13" s="25">
+        <v>80.203751249999996</v>
+      </c>
+      <c r="E13" s="25">
+        <v>68.909969700000005</v>
+      </c>
+      <c r="F13" s="25">
+        <v>336.73053019999998</v>
+      </c>
+      <c r="G13" s="25">
+        <v>87.361183130000001</v>
+      </c>
+      <c r="H13" s="25">
+        <v>657.25965210000004</v>
+      </c>
+      <c r="I13" s="25">
+        <v>255.00832270000001</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -10518,28 +10521,28 @@
         <v>12</v>
       </c>
       <c r="B14" s="9">
-        <v>2404</v>
+        <v>2726</v>
       </c>
       <c r="C14" s="9">
-        <v>2404</v>
-      </c>
-      <c r="D14" s="8">
-        <v>81</v>
-      </c>
-      <c r="E14" s="8">
-        <v>70</v>
-      </c>
-      <c r="F14" s="8">
-        <v>318</v>
-      </c>
-      <c r="G14" s="8">
-        <v>87</v>
-      </c>
-      <c r="H14" s="8">
-        <v>657</v>
-      </c>
-      <c r="I14" s="8">
-        <v>255</v>
+        <v>2589</v>
+      </c>
+      <c r="D14" s="25">
+        <v>81.292076750000007</v>
+      </c>
+      <c r="E14" s="25">
+        <v>69.745811709999998</v>
+      </c>
+      <c r="F14" s="25">
+        <v>350.37185410000001</v>
+      </c>
+      <c r="G14" s="25">
+        <v>87.505193180000006</v>
+      </c>
+      <c r="H14" s="25">
+        <v>683.19788659999995</v>
+      </c>
+      <c r="I14" s="25">
+        <v>259.29791369999998</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -10547,28 +10550,28 @@
         <v>13</v>
       </c>
       <c r="B15" s="9">
-        <v>2476</v>
+        <v>2970</v>
       </c>
       <c r="C15" s="9">
-        <v>2476</v>
-      </c>
-      <c r="D15" s="8">
-        <v>82</v>
-      </c>
-      <c r="E15" s="8">
-        <v>70</v>
-      </c>
-      <c r="F15" s="8">
-        <v>318</v>
-      </c>
-      <c r="G15" s="8">
-        <v>87</v>
-      </c>
-      <c r="H15" s="8">
-        <v>683</v>
-      </c>
-      <c r="I15" s="8">
-        <v>259</v>
+        <v>2696</v>
+      </c>
+      <c r="D15" s="25">
+        <v>82.145842270000003</v>
+      </c>
+      <c r="E15" s="25">
+        <v>70.399311190000006</v>
+      </c>
+      <c r="F15" s="25">
+        <v>359.74853630000001</v>
+      </c>
+      <c r="G15" s="25">
+        <v>87.588019619999997</v>
+      </c>
+      <c r="H15" s="25">
+        <v>701.87683049999998</v>
+      </c>
+      <c r="I15" s="25">
+        <v>262.68195250000002</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -10576,28 +10579,28 @@
         <v>14</v>
       </c>
       <c r="B16" s="9">
-        <v>2726</v>
+        <v>3214</v>
       </c>
       <c r="C16" s="9">
-        <v>2589</v>
-      </c>
-      <c r="D16" s="8">
-        <v>83</v>
-      </c>
-      <c r="E16" s="8">
-        <v>71</v>
-      </c>
-      <c r="F16" s="8">
-        <v>318</v>
-      </c>
-      <c r="G16" s="8">
-        <v>87</v>
-      </c>
-      <c r="H16" s="8">
-        <v>702</v>
-      </c>
-      <c r="I16" s="8">
-        <v>263</v>
+        <v>2803</v>
+      </c>
+      <c r="D16" s="25">
+        <v>82.815601060000006</v>
+      </c>
+      <c r="E16" s="25">
+        <v>70.910246950000001</v>
+      </c>
+      <c r="F16" s="25">
+        <v>366.05140410000001</v>
+      </c>
+      <c r="G16" s="25">
+        <v>87.6356392</v>
+      </c>
+      <c r="H16" s="25">
+        <v>715.06050809999999</v>
+      </c>
+      <c r="I16" s="25">
+        <v>265.34575009999998</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -10605,28 +10608,28 @@
         <v>15</v>
       </c>
       <c r="B17" s="9">
-        <v>2968</v>
+        <v>3458</v>
       </c>
       <c r="C17" s="9">
-        <v>2701</v>
-      </c>
-      <c r="D17" s="8">
-        <v>83</v>
-      </c>
-      <c r="E17" s="8">
-        <v>71</v>
-      </c>
-      <c r="F17" s="8">
-        <v>318</v>
-      </c>
-      <c r="G17" s="8">
-        <v>87</v>
-      </c>
-      <c r="H17" s="8">
-        <v>715</v>
-      </c>
-      <c r="I17" s="8">
-        <v>265</v>
+        <v>2910</v>
+      </c>
+      <c r="D17" s="25">
+        <v>83.341010940000004</v>
+      </c>
+      <c r="E17" s="25">
+        <v>71.309719869999995</v>
+      </c>
+      <c r="F17" s="25">
+        <v>370.22471469999999</v>
+      </c>
+      <c r="G17" s="25">
+        <v>87.663011429999997</v>
+      </c>
+      <c r="H17" s="25">
+        <v>724.23416829999996</v>
+      </c>
+      <c r="I17" s="25">
+        <v>267.43903360000002</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -10634,28 +10637,28 @@
         <v>16</v>
       </c>
       <c r="B18" s="9">
-        <v>3218</v>
+        <v>3702</v>
       </c>
       <c r="C18" s="9">
-        <v>2806</v>
-      </c>
-      <c r="D18" s="8">
-        <v>84</v>
-      </c>
-      <c r="E18" s="8">
-        <v>72</v>
-      </c>
-      <c r="F18" s="8">
-        <v>318</v>
-      </c>
-      <c r="G18" s="8">
-        <v>87</v>
-      </c>
-      <c r="H18" s="8">
-        <v>724</v>
-      </c>
-      <c r="I18" s="8">
-        <v>267</v>
+        <v>3017</v>
+      </c>
+      <c r="D18" s="25">
+        <v>83.753182530000004</v>
+      </c>
+      <c r="E18" s="25">
+        <v>71.622046060000002</v>
+      </c>
+      <c r="F18" s="25">
+        <v>372.96047190000002</v>
+      </c>
+      <c r="G18" s="25">
+        <v>87.678743370000007</v>
+      </c>
+      <c r="H18" s="25">
+        <v>730.5545085</v>
+      </c>
+      <c r="I18" s="25">
+        <v>269.08181949999999</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -10663,28 +10666,28 @@
         <v>17</v>
       </c>
       <c r="B19" s="9">
-        <v>3460</v>
+        <v>3946</v>
       </c>
       <c r="C19" s="9">
-        <v>2911</v>
-      </c>
-      <c r="D19" s="8">
-        <v>84</v>
-      </c>
-      <c r="E19" s="8">
-        <v>72</v>
-      </c>
-      <c r="F19" s="8">
-        <v>318</v>
-      </c>
-      <c r="G19" s="8">
-        <v>87</v>
-      </c>
-      <c r="H19" s="8">
-        <v>731</v>
-      </c>
-      <c r="I19" s="8">
-        <v>269</v>
+        <v>3124</v>
+      </c>
+      <c r="D19" s="25">
+        <v>84.076521349999993</v>
+      </c>
+      <c r="E19" s="25">
+        <v>71.866236950000001</v>
+      </c>
+      <c r="F19" s="25">
+        <v>374.74211539999999</v>
+      </c>
+      <c r="G19" s="25">
+        <v>87.687784530000002</v>
+      </c>
+      <c r="H19" s="25">
+        <v>734.87930259999996</v>
+      </c>
+      <c r="I19" s="25">
+        <v>270.36973619999998</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -10692,28 +10695,28 @@
         <v>18</v>
       </c>
       <c r="B20" s="9">
-        <v>3710</v>
+        <v>4190</v>
       </c>
       <c r="C20" s="9">
-        <v>3024</v>
-      </c>
-      <c r="D20" s="8">
-        <v>84</v>
-      </c>
-      <c r="E20" s="8">
-        <v>72</v>
-      </c>
-      <c r="F20" s="8">
-        <v>318</v>
-      </c>
-      <c r="G20" s="8">
-        <v>87</v>
-      </c>
-      <c r="H20" s="8">
-        <v>735</v>
-      </c>
-      <c r="I20" s="8">
-        <v>270</v>
+        <v>3231</v>
+      </c>
+      <c r="D20" s="25">
+        <v>84.330172989999994</v>
+      </c>
+      <c r="E20" s="25">
+        <v>72.057156539999994</v>
+      </c>
+      <c r="F20" s="25">
+        <v>375.89743859999999</v>
+      </c>
+      <c r="G20" s="25">
+        <v>87.69298028</v>
+      </c>
+      <c r="H20" s="25">
+        <v>737.82476859999997</v>
+      </c>
+      <c r="I20" s="25">
+        <v>271.37863440000001</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -10721,28 +10724,28 @@
         <v>19</v>
       </c>
       <c r="B21" s="9">
-        <v>3944</v>
+        <v>4434</v>
       </c>
       <c r="C21" s="9">
-        <v>3128</v>
-      </c>
-      <c r="D21" s="8">
-        <v>85</v>
-      </c>
-      <c r="E21" s="8">
-        <v>72</v>
-      </c>
-      <c r="F21" s="8">
-        <v>318</v>
-      </c>
-      <c r="G21" s="8">
-        <v>87</v>
-      </c>
-      <c r="H21" s="8">
-        <v>738</v>
-      </c>
-      <c r="I21" s="8">
-        <v>271</v>
+        <v>3338</v>
+      </c>
+      <c r="D21" s="25">
+        <v>84.52915668</v>
+      </c>
+      <c r="E21" s="25">
+        <v>72.206426199999996</v>
+      </c>
+      <c r="F21" s="25">
+        <v>376.6445387</v>
+      </c>
+      <c r="G21" s="25">
+        <v>87.695966100000007</v>
+      </c>
+      <c r="H21" s="25">
+        <v>739.82442160000005</v>
+      </c>
+      <c r="I21" s="25">
+        <v>272.16846939999999</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -10750,28 +10753,28 @@
         <v>20</v>
       </c>
       <c r="B22" s="9">
-        <v>4194</v>
+        <v>4434</v>
       </c>
       <c r="C22" s="9">
-        <v>3233</v>
-      </c>
-      <c r="D22" s="8">
-        <v>85</v>
-      </c>
-      <c r="E22" s="8">
-        <v>72</v>
-      </c>
-      <c r="F22" s="8">
-        <v>318</v>
-      </c>
-      <c r="G22" s="8">
-        <v>87</v>
-      </c>
-      <c r="H22" s="8">
-        <v>740</v>
-      </c>
-      <c r="I22" s="8">
-        <v>272</v>
+        <v>3338</v>
+      </c>
+      <c r="D22" s="25">
+        <v>84.685254659999998</v>
+      </c>
+      <c r="E22" s="25">
+        <v>72.323132049999998</v>
+      </c>
+      <c r="F22" s="25">
+        <v>377.12678940000001</v>
+      </c>
+      <c r="G22" s="25">
+        <v>87.697681919999994</v>
+      </c>
+      <c r="H22" s="25">
+        <v>741.17902609999999</v>
+      </c>
+      <c r="I22" s="25">
+        <v>272.78650670000002</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -10779,28 +10782,28 @@
         <v>21</v>
       </c>
       <c r="B23" s="9">
-        <v>4436</v>
+        <v>4434</v>
       </c>
       <c r="C23" s="9">
-        <v>3346</v>
-      </c>
-      <c r="D23" s="8">
-        <v>85</v>
-      </c>
-      <c r="E23" s="8">
-        <v>72</v>
-      </c>
-      <c r="F23" s="8">
-        <v>318</v>
-      </c>
-      <c r="G23" s="8">
-        <v>87</v>
-      </c>
-      <c r="H23" s="8">
-        <v>741</v>
-      </c>
-      <c r="I23" s="8">
-        <v>273</v>
+        <v>3338</v>
+      </c>
+      <c r="D23" s="25">
+        <v>84.807709819999999</v>
+      </c>
+      <c r="E23" s="25">
+        <v>72.414378009999993</v>
+      </c>
+      <c r="F23" s="25">
+        <v>377.43771950000001</v>
+      </c>
+      <c r="G23" s="25">
+        <v>87.698667920000005</v>
+      </c>
+      <c r="H23" s="25">
+        <v>742.09531300000003</v>
+      </c>
+      <c r="I23" s="25">
+        <v>273.26993119999997</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -10808,28 +10811,28 @@
         <v>22</v>
       </c>
       <c r="B24" s="9">
-        <v>4428</v>
+        <v>4434</v>
       </c>
       <c r="C24" s="9">
-        <v>3337</v>
-      </c>
-      <c r="D24" s="8">
-        <v>85</v>
-      </c>
-      <c r="E24" s="8">
-        <v>72</v>
-      </c>
-      <c r="F24" s="8">
-        <v>318</v>
-      </c>
-      <c r="G24" s="8">
-        <v>87</v>
-      </c>
-      <c r="H24" s="8">
-        <v>742</v>
-      </c>
-      <c r="I24" s="8">
-        <v>273</v>
+        <v>3338</v>
+      </c>
+      <c r="D24" s="25">
+        <v>84.903772989999993</v>
+      </c>
+      <c r="E24" s="25">
+        <v>72.485718270000007</v>
+      </c>
+      <c r="F24" s="25">
+        <v>377.6380408</v>
+      </c>
+      <c r="G24" s="25">
+        <v>87.699234520000005</v>
+      </c>
+      <c r="H24" s="25">
+        <v>742.71449489999998</v>
+      </c>
+      <c r="I24" s="25">
+        <v>273.64795079999999</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -10837,28 +10840,28 @@
         <v>23</v>
       </c>
       <c r="B25" s="9">
-        <v>4436</v>
+        <v>4434</v>
       </c>
       <c r="C25" s="9">
-        <v>3329</v>
-      </c>
-      <c r="D25" s="8">
-        <v>85</v>
-      </c>
-      <c r="E25" s="8">
-        <v>73</v>
-      </c>
-      <c r="F25" s="8">
-        <v>318</v>
-      </c>
-      <c r="G25" s="8">
-        <v>87</v>
-      </c>
-      <c r="H25" s="8">
-        <v>743</v>
-      </c>
-      <c r="I25" s="8">
-        <v>274</v>
+        <v>3338</v>
+      </c>
+      <c r="D25" s="25">
+        <v>84.979132269999994</v>
+      </c>
+      <c r="E25" s="25">
+        <v>72.541495350000005</v>
+      </c>
+      <c r="F25" s="25">
+        <v>377.76703859999998</v>
+      </c>
+      <c r="G25" s="25">
+        <v>87.699560120000001</v>
+      </c>
+      <c r="H25" s="25">
+        <v>743.13262640000005</v>
+      </c>
+      <c r="I25" s="25">
+        <v>273.94347959999999</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -10866,28 +10869,28 @@
         <v>24</v>
       </c>
       <c r="B26" s="9">
-        <v>4435</v>
+        <v>4434</v>
       </c>
       <c r="C26" s="9">
-        <v>3345</v>
-      </c>
-      <c r="D26" s="8">
-        <v>85</v>
-      </c>
-      <c r="E26" s="8">
-        <v>73</v>
-      </c>
-      <c r="F26" s="8">
-        <v>318</v>
-      </c>
-      <c r="G26" s="8">
-        <v>87</v>
-      </c>
-      <c r="H26" s="8">
-        <v>743</v>
-      </c>
-      <c r="I26" s="8">
-        <v>274</v>
+        <v>3338</v>
+      </c>
+      <c r="D26" s="25">
+        <v>85.038249829999998</v>
+      </c>
+      <c r="E26" s="25">
+        <v>72.585104419999993</v>
+      </c>
+      <c r="F26" s="25">
+        <v>377.85008140000002</v>
+      </c>
+      <c r="G26" s="25">
+        <v>87.699747220000006</v>
+      </c>
+      <c r="H26" s="25">
+        <v>743.41486090000001</v>
+      </c>
+      <c r="I26" s="25">
+        <v>274.17447720000001</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -10895,28 +10898,28 @@
         <v>25</v>
       </c>
       <c r="B27" s="9">
-        <v>4443</v>
+        <v>4434</v>
       </c>
       <c r="C27" s="9">
-        <v>3344</v>
-      </c>
-      <c r="D27" s="8">
-        <v>85</v>
-      </c>
-      <c r="E27" s="8">
-        <v>73</v>
-      </c>
-      <c r="F27" s="8">
-        <v>318</v>
-      </c>
-      <c r="G27" s="8">
-        <v>87</v>
-      </c>
-      <c r="H27" s="8">
-        <v>743</v>
-      </c>
-      <c r="I27" s="8">
-        <v>274</v>
+        <v>3338</v>
+      </c>
+      <c r="D27" s="25">
+        <v>85.084626159999999</v>
+      </c>
+      <c r="E27" s="25">
+        <v>72.619199980000005</v>
+      </c>
+      <c r="F27" s="25">
+        <v>377.9035298</v>
+      </c>
+      <c r="G27" s="25">
+        <v>87.699854740000006</v>
+      </c>
+      <c r="H27" s="25">
+        <v>743.60530800000004</v>
+      </c>
+      <c r="I27" s="25">
+        <v>274.35500910000002</v>
       </c>
     </row>
   </sheetData>
@@ -11709,7 +11712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>